<commit_message>
intro parse working going to add 1st foco internal node for analysis
</commit_message>
<xml_diff>
--- a/R/data_input/2013-2021 WNV Surveillance Trap Consolidation (from Kaitlynn).xlsx
+++ b/R/data_input/2013-2021 WNV Surveillance Trap Consolidation (from Kaitlynn).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Programming Directory/Ebel Lab/WNV-Foco-nextstrain2/R/data_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDAE9C6-B969-2648-B0DB-5008916EFE03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01D52B2-F202-DC4F-8B30-82AE898C2EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25440" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9529,8 +9529,8 @@
   </sheetPr>
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9855,7 +9855,7 @@
         <v>52</v>
       </c>
       <c r="B25" s="67" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C25" s="68" t="s">
         <v>53</v>
@@ -9881,7 +9881,7 @@
         <v>56</v>
       </c>
       <c r="B27" s="69" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C27" s="68" t="s">
         <v>57</v>
@@ -9959,7 +9959,7 @@
         <v>68</v>
       </c>
       <c r="B33" s="67" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C33" s="68" t="s">
         <v>69</v>
@@ -25373,7 +25373,7 @@
   </sheetPr>
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>

</xml_diff>